<commit_message>
Creating standalone and finishing documentation
</commit_message>
<xml_diff>
--- a/leaders.xlsx
+++ b/leaders.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dav_r\PycharmProjects\Teams\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dav_r\Documents\Orientation-Teams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33BC4CF4-6526-458F-B1BE-FF1D53A17CF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E9F770-6F94-4458-A8E0-5BB7E5C6BEB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8540" yWindow="760" windowWidth="9000" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18220" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Leaders" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -71,16 +71,54 @@
   </si>
   <si>
     <t>team 2</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>davrene11@gmail.com</t>
+  </si>
+  <si>
+    <t>email1</t>
+  </si>
+  <si>
+    <t>email2</t>
+  </si>
+  <si>
+    <t>email3</t>
+  </si>
+  <si>
+    <t>email4</t>
+  </si>
+  <si>
+    <t>email5</t>
+  </si>
+  <si>
+    <t>email6</t>
+  </si>
+  <si>
+    <t>email7</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -103,13 +141,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -388,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -399,9 +440,10 @@
     <col min="1" max="1" width="16.453125" customWidth="1"/>
     <col min="2" max="2" width="13.36328125" customWidth="1"/>
     <col min="3" max="3" width="17.90625" customWidth="1"/>
+    <col min="4" max="4" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -411,54 +453,126 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{5BF80E0A-C9AC-4A47-A7E1-566A02FBADDD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>